<commit_message>
Atualizar links e imagens em várias páginas; melhorar estilo de exibição das imagens nos cards de curso
</commit_message>
<xml_diff>
--- a/src/imgs/planilha/Planilha_Controle_Financeiro_Capacita.xlsx
+++ b/src/imgs/planilha/Planilha_Controle_Financeiro_Capacita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trambuco.DESKTOP-5LJKETL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822CB475-FC49-41E0-A5E5-8044EDDE4684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4B83AB-D65F-48D5-BFFA-39F9F562AB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -843,6 +843,27 @@
     <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -853,9 +874,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,29 +894,11 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1239,116 +1239,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>123264</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>44821</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1322293</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>145674</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagem 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C77432A-AFD7-4B27-A0A6-C5741B7A0FAE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="-1307" t="36850" r="-10346" b="2946"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="123264" y="179292"/>
-          <a:ext cx="2902323" cy="1703294"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagem 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F5E0BF-F088-4A26-96E2-D31D47E2B481}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="209550" y="133350"/>
-          <a:ext cx="1495425" cy="771525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1677,7 +1567,7 @@
   <dimension ref="A1:P126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1792,11 +1682,11 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1814,9 +1704,9 @@
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="7" t="s">
         <v>2</v>
       </c>
@@ -1834,9 +1724,9 @@
       <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="7" t="s">
         <v>3</v>
       </c>
@@ -1854,9 +1744,9 @@
       <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
@@ -1874,9 +1764,9 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="7" t="s">
         <v>74</v>
       </c>
@@ -1894,9 +1784,9 @@
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="7" t="s">
         <v>75</v>
       </c>
@@ -1914,9 +1804,9 @@
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="7" t="s">
         <v>73</v>
       </c>
@@ -1934,9 +1824,9 @@
       <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1952,9 +1842,9 @@
       <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="11" t="s">
         <v>49</v>
       </c>
@@ -2008,11 +1898,11 @@
       </c>
     </row>
     <row r="16" spans="1:16" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
@@ -2028,9 +1918,9 @@
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
@@ -2046,9 +1936,9 @@
       <c r="P17" s="16"/>
     </row>
     <row r="18" spans="1:16" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="13"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -2064,11 +1954,11 @@
       <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="7" t="s">
         <v>24</v>
       </c>
@@ -2086,9 +1976,9 @@
       <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="7" t="s">
         <v>25</v>
       </c>
@@ -2106,9 +1996,9 @@
       <c r="P20" s="8"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="7" t="s">
         <v>76</v>
       </c>
@@ -2126,9 +2016,9 @@
       <c r="P21" s="8"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="7" t="s">
         <v>47</v>
       </c>
@@ -2146,9 +2036,9 @@
       <c r="P22" s="8"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="7" t="s">
         <v>73</v>
       </c>
@@ -2166,9 +2056,9 @@
       <c r="P23" s="8"/>
     </row>
     <row r="24" spans="1:16" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="9"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -2184,9 +2074,9 @@
       <c r="P24" s="17"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="11" t="s">
         <v>49</v>
       </c>
@@ -2240,9 +2130,9 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="51"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="18"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -2258,9 +2148,9 @@
       <c r="P26" s="16"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="19" t="s">
         <v>94</v>
       </c>
@@ -2314,11 +2204,11 @@
       </c>
     </row>
     <row r="28" spans="1:16" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="13"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
@@ -2334,9 +2224,9 @@
       <c r="P28" s="14"/>
     </row>
     <row r="29" spans="1:16" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
       <c r="D29" s="15"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -2352,9 +2242,9 @@
       <c r="P29" s="16"/>
     </row>
     <row r="30" spans="1:16" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="65"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
       <c r="D30" s="13"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -2370,11 +2260,11 @@
       <c r="P30" s="6"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="58" t="s">
+      <c r="B31" s="50"/>
+      <c r="C31" s="49" t="s">
         <v>50</v>
       </c>
       <c r="D31" s="21" t="s">
@@ -2394,9 +2284,9 @@
       <c r="P31" s="22"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="58"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="49"/>
       <c r="D32" s="21" t="s">
         <v>10</v>
       </c>
@@ -2414,9 +2304,9 @@
       <c r="P32" s="22"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="58"/>
+      <c r="A33" s="51"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="21" t="s">
         <v>11</v>
       </c>
@@ -2434,9 +2324,9 @@
       <c r="P33" s="22"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="58"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="21" t="s">
         <v>77</v>
       </c>
@@ -2454,9 +2344,9 @@
       <c r="P34" s="22"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="59"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="58"/>
+      <c r="A35" s="51"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="21" t="s">
         <v>12</v>
       </c>
@@ -2474,9 +2364,9 @@
       <c r="P35" s="22"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="59"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="58"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="21" t="s">
         <v>13</v>
       </c>
@@ -2494,8 +2384,8 @@
       <c r="P36" s="22"/>
     </row>
     <row r="37" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="59"/>
-      <c r="B37" s="59"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="37"/>
       <c r="D37" s="18"/>
       <c r="E37" s="16"/>
@@ -2512,9 +2402,9 @@
       <c r="P37" s="16"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="59"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="58" t="s">
+      <c r="A38" s="51"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="49" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="21" t="s">
@@ -2534,9 +2424,9 @@
       <c r="P38" s="22"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="59"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="58"/>
+      <c r="A39" s="51"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="21" t="s">
         <v>62</v>
       </c>
@@ -2554,9 +2444,9 @@
       <c r="P39" s="22"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="58"/>
+      <c r="A40" s="51"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="21" t="s">
         <v>32</v>
       </c>
@@ -2574,8 +2464,8 @@
       <c r="P40" s="22"/>
     </row>
     <row r="41" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="59"/>
-      <c r="B41" s="59"/>
+      <c r="A41" s="51"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="37"/>
       <c r="D41" s="18"/>
       <c r="E41" s="16"/>
@@ -2592,9 +2482,9 @@
       <c r="P41" s="16"/>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="59"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="60" t="s">
+      <c r="A42" s="51"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="64" t="s">
         <v>57</v>
       </c>
       <c r="D42" s="21" t="s">
@@ -2614,9 +2504,9 @@
       <c r="P42" s="22"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="59"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="61"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="21" t="s">
         <v>79</v>
       </c>
@@ -2634,8 +2524,8 @@
       <c r="P43" s="22"/>
     </row>
     <row r="44" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="59"/>
-      <c r="B44" s="59"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="37"/>
       <c r="D44" s="18"/>
       <c r="E44" s="16"/>
@@ -2652,9 +2542,9 @@
       <c r="P44" s="16"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="59"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="58" t="s">
+      <c r="A45" s="51"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="49" t="s">
         <v>59</v>
       </c>
       <c r="D45" s="21" t="s">
@@ -2674,9 +2564,9 @@
       <c r="P45" s="22"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="59"/>
-      <c r="B46" s="59"/>
-      <c r="C46" s="58"/>
+      <c r="A46" s="51"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="21" t="s">
         <v>18</v>
       </c>
@@ -2694,9 +2584,9 @@
       <c r="P46" s="22"/>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="59"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="58"/>
+      <c r="A47" s="51"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="49"/>
       <c r="D47" s="21" t="s">
         <v>60</v>
       </c>
@@ -2714,8 +2604,8 @@
       <c r="P47" s="22"/>
     </row>
     <row r="48" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="59"/>
-      <c r="B48" s="59"/>
+      <c r="A48" s="51"/>
+      <c r="B48" s="51"/>
       <c r="C48" s="37"/>
       <c r="D48" s="18"/>
       <c r="E48" s="16"/>
@@ -2732,9 +2622,9 @@
       <c r="P48" s="16"/>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="59"/>
-      <c r="B49" s="59"/>
-      <c r="C49" s="58" t="s">
+      <c r="A49" s="51"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="49" t="s">
         <v>58</v>
       </c>
       <c r="D49" s="21" t="s">
@@ -2754,9 +2644,9 @@
       <c r="P49" s="22"/>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="59"/>
-      <c r="B50" s="59"/>
-      <c r="C50" s="58"/>
+      <c r="A50" s="51"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="49"/>
       <c r="D50" s="21" t="s">
         <v>16</v>
       </c>
@@ -2774,8 +2664,8 @@
       <c r="P50" s="22"/>
     </row>
     <row r="51" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="59"/>
-      <c r="B51" s="59"/>
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
       <c r="C51" s="37"/>
       <c r="D51" s="18"/>
       <c r="E51" s="43"/>
@@ -2792,8 +2682,8 @@
       <c r="P51" s="16"/>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="59"/>
-      <c r="B52" s="59"/>
+      <c r="A52" s="51"/>
+      <c r="B52" s="51"/>
       <c r="C52" s="38" t="s">
         <v>73</v>
       </c>
@@ -2814,8 +2704,8 @@
       <c r="P52" s="22"/>
     </row>
     <row r="53" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="59"/>
-      <c r="B53" s="59"/>
+      <c r="A53" s="51"/>
+      <c r="B53" s="51"/>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
       <c r="E53" s="16"/>
@@ -2832,8 +2722,8 @@
       <c r="P53" s="16"/>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="59"/>
-      <c r="B54" s="59"/>
+      <c r="A54" s="51"/>
+      <c r="B54" s="51"/>
       <c r="C54" s="23" t="s">
         <v>81</v>
       </c>
@@ -2888,8 +2778,8 @@
       </c>
     </row>
     <row r="55" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="59"/>
-      <c r="B55" s="59"/>
+      <c r="A55" s="51"/>
+      <c r="B55" s="51"/>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
       <c r="E55" s="16"/>
@@ -2906,8 +2796,8 @@
       <c r="P55" s="16"/>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="59"/>
-      <c r="B56" s="59"/>
+      <c r="A56" s="51"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="23" t="s">
         <v>94</v>
       </c>
@@ -2978,11 +2868,11 @@
       <c r="P57" s="16"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="59"/>
-      <c r="C58" s="58" t="s">
+      <c r="B58" s="51"/>
+      <c r="C58" s="49" t="s">
         <v>50</v>
       </c>
       <c r="D58" s="21" t="s">
@@ -3002,9 +2892,9 @@
       <c r="P58" s="22"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A59" s="59"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="58"/>
+      <c r="A59" s="51"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="21" t="s">
         <v>7</v>
       </c>
@@ -3022,9 +2912,9 @@
       <c r="P59" s="22"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="59"/>
-      <c r="B60" s="59"/>
-      <c r="C60" s="58"/>
+      <c r="A60" s="51"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="21" t="s">
         <v>8</v>
       </c>
@@ -3042,9 +2932,9 @@
       <c r="P60" s="22"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="59"/>
-      <c r="B61" s="59"/>
-      <c r="C61" s="58"/>
+      <c r="A61" s="51"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="21" t="s">
         <v>21</v>
       </c>
@@ -3062,9 +2952,9 @@
       <c r="P61" s="22"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A62" s="59"/>
-      <c r="B62" s="59"/>
-      <c r="C62" s="58"/>
+      <c r="A62" s="51"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="21" t="s">
         <v>9</v>
       </c>
@@ -3082,9 +2972,9 @@
       <c r="P62" s="22"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A63" s="59"/>
-      <c r="B63" s="59"/>
-      <c r="C63" s="58"/>
+      <c r="A63" s="51"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="49"/>
       <c r="D63" s="21" t="s">
         <v>72</v>
       </c>
@@ -3102,9 +2992,9 @@
       <c r="P63" s="22"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A64" s="59"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="58"/>
+      <c r="A64" s="51"/>
+      <c r="B64" s="51"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="21" t="s">
         <v>61</v>
       </c>
@@ -3122,8 +3012,8 @@
       <c r="P64" s="22"/>
     </row>
     <row r="65" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="59"/>
-      <c r="B65" s="59"/>
+      <c r="A65" s="51"/>
+      <c r="B65" s="51"/>
       <c r="C65" s="37"/>
       <c r="D65" s="18"/>
       <c r="E65" s="26"/>
@@ -3140,9 +3030,9 @@
       <c r="P65" s="26"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="59"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="58" t="s">
+      <c r="A66" s="51"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="49" t="s">
         <v>22</v>
       </c>
       <c r="D66" s="21" t="s">
@@ -3162,9 +3052,9 @@
       <c r="P66" s="22"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" s="59"/>
-      <c r="B67" s="59"/>
-      <c r="C67" s="58"/>
+      <c r="A67" s="51"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="49"/>
       <c r="D67" s="21" t="s">
         <v>52</v>
       </c>
@@ -3182,9 +3072,9 @@
       <c r="P67" s="22"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A68" s="59"/>
-      <c r="B68" s="59"/>
-      <c r="C68" s="58"/>
+      <c r="A68" s="51"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="21" t="s">
         <v>53</v>
       </c>
@@ -3202,9 +3092,9 @@
       <c r="P68" s="22"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A69" s="59"/>
-      <c r="B69" s="59"/>
-      <c r="C69" s="58"/>
+      <c r="A69" s="51"/>
+      <c r="B69" s="51"/>
+      <c r="C69" s="49"/>
       <c r="D69" s="21" t="s">
         <v>32</v>
       </c>
@@ -3222,8 +3112,8 @@
       <c r="P69" s="22"/>
     </row>
     <row r="70" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="59"/>
-      <c r="B70" s="59"/>
+      <c r="A70" s="51"/>
+      <c r="B70" s="51"/>
       <c r="C70" s="39"/>
       <c r="D70" s="18"/>
       <c r="E70" s="26"/>
@@ -3240,9 +3130,9 @@
       <c r="P70" s="26"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A71" s="59"/>
-      <c r="B71" s="59"/>
-      <c r="C71" s="58" t="s">
+      <c r="A71" s="51"/>
+      <c r="B71" s="51"/>
+      <c r="C71" s="49" t="s">
         <v>54</v>
       </c>
       <c r="D71" s="21" t="s">
@@ -3262,9 +3152,9 @@
       <c r="P71" s="22"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="59"/>
-      <c r="B72" s="59"/>
-      <c r="C72" s="58"/>
+      <c r="A72" s="51"/>
+      <c r="B72" s="51"/>
+      <c r="C72" s="49"/>
       <c r="D72" s="21" t="s">
         <v>55</v>
       </c>
@@ -3282,9 +3172,9 @@
       <c r="P72" s="22"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A73" s="59"/>
-      <c r="B73" s="59"/>
-      <c r="C73" s="58"/>
+      <c r="A73" s="51"/>
+      <c r="B73" s="51"/>
+      <c r="C73" s="49"/>
       <c r="D73" s="21" t="s">
         <v>56</v>
       </c>
@@ -3302,8 +3192,8 @@
       <c r="P73" s="22"/>
     </row>
     <row r="74" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="59"/>
-      <c r="B74" s="59"/>
+      <c r="A74" s="51"/>
+      <c r="B74" s="51"/>
       <c r="C74" s="39"/>
       <c r="D74" s="18"/>
       <c r="E74" s="26"/>
@@ -3320,8 +3210,8 @@
       <c r="P74" s="26"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A75" s="59"/>
-      <c r="B75" s="59"/>
+      <c r="A75" s="51"/>
+      <c r="B75" s="51"/>
       <c r="C75" s="38" t="s">
         <v>57</v>
       </c>
@@ -3342,8 +3232,8 @@
       <c r="P75" s="22"/>
     </row>
     <row r="76" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="59"/>
-      <c r="B76" s="59"/>
+      <c r="A76" s="51"/>
+      <c r="B76" s="51"/>
       <c r="C76" s="39"/>
       <c r="D76" s="18"/>
       <c r="E76" s="26"/>
@@ -3360,9 +3250,9 @@
       <c r="P76" s="26"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A77" s="59"/>
-      <c r="B77" s="59"/>
-      <c r="C77" s="58" t="s">
+      <c r="A77" s="51"/>
+      <c r="B77" s="51"/>
+      <c r="C77" s="49" t="s">
         <v>82</v>
       </c>
       <c r="D77" s="21" t="s">
@@ -3382,9 +3272,9 @@
       <c r="P77" s="22"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A78" s="59"/>
-      <c r="B78" s="59"/>
-      <c r="C78" s="58"/>
+      <c r="A78" s="51"/>
+      <c r="B78" s="51"/>
+      <c r="C78" s="49"/>
       <c r="D78" s="21" t="s">
         <v>63</v>
       </c>
@@ -3402,9 +3292,9 @@
       <c r="P78" s="22"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A79" s="59"/>
-      <c r="B79" s="59"/>
-      <c r="C79" s="58"/>
+      <c r="A79" s="51"/>
+      <c r="B79" s="51"/>
+      <c r="C79" s="49"/>
       <c r="D79" s="21" t="s">
         <v>64</v>
       </c>
@@ -3422,9 +3312,9 @@
       <c r="P79" s="22"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A80" s="59"/>
-      <c r="B80" s="59"/>
-      <c r="C80" s="58"/>
+      <c r="A80" s="51"/>
+      <c r="B80" s="51"/>
+      <c r="C80" s="49"/>
       <c r="D80" s="21" t="s">
         <v>20</v>
       </c>
@@ -3442,9 +3332,9 @@
       <c r="P80" s="22"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A81" s="59"/>
-      <c r="B81" s="59"/>
-      <c r="C81" s="58"/>
+      <c r="A81" s="51"/>
+      <c r="B81" s="51"/>
+      <c r="C81" s="49"/>
       <c r="D81" s="21" t="s">
         <v>19</v>
       </c>
@@ -3462,8 +3352,8 @@
       <c r="P81" s="22"/>
     </row>
     <row r="82" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="59"/>
-      <c r="B82" s="59"/>
+      <c r="A82" s="51"/>
+      <c r="B82" s="51"/>
       <c r="C82" s="27"/>
       <c r="D82" s="18"/>
       <c r="E82" s="16"/>
@@ -3480,8 +3370,8 @@
       <c r="P82" s="16"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A83" s="59"/>
-      <c r="B83" s="59"/>
+      <c r="A83" s="51"/>
+      <c r="B83" s="51"/>
       <c r="C83" s="28" t="s">
         <v>84</v>
       </c>
@@ -3536,8 +3426,8 @@
       </c>
     </row>
     <row r="84" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="59"/>
-      <c r="B84" s="59"/>
+      <c r="A84" s="51"/>
+      <c r="B84" s="51"/>
       <c r="C84" s="18"/>
       <c r="D84" s="18"/>
       <c r="E84" s="16"/>
@@ -3554,8 +3444,8 @@
       <c r="P84" s="16"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A85" s="59"/>
-      <c r="B85" s="59"/>
+      <c r="A85" s="51"/>
+      <c r="B85" s="51"/>
       <c r="C85" s="23" t="s">
         <v>94</v>
       </c>
@@ -3626,11 +3516,11 @@
       <c r="P86" s="16"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A87" s="59" t="s">
+      <c r="A87" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="B87" s="59"/>
-      <c r="C87" s="58" t="s">
+      <c r="B87" s="51"/>
+      <c r="C87" s="49" t="s">
         <v>57</v>
       </c>
       <c r="D87" s="21" t="s">
@@ -3650,9 +3540,9 @@
       <c r="P87" s="22"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A88" s="59"/>
-      <c r="B88" s="59"/>
-      <c r="C88" s="58"/>
+      <c r="A88" s="51"/>
+      <c r="B88" s="51"/>
+      <c r="C88" s="49"/>
       <c r="D88" s="21" t="s">
         <v>29</v>
       </c>
@@ -3670,9 +3560,9 @@
       <c r="P88" s="22"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A89" s="59"/>
-      <c r="B89" s="59"/>
-      <c r="C89" s="58"/>
+      <c r="A89" s="51"/>
+      <c r="B89" s="51"/>
+      <c r="C89" s="49"/>
       <c r="D89" s="21" t="s">
         <v>65</v>
       </c>
@@ -3690,8 +3580,8 @@
       <c r="P89" s="22"/>
     </row>
     <row r="90" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="59"/>
-      <c r="B90" s="59"/>
+      <c r="A90" s="51"/>
+      <c r="B90" s="51"/>
       <c r="C90" s="39"/>
       <c r="D90" s="18"/>
       <c r="E90" s="26"/>
@@ -3708,9 +3598,9 @@
       <c r="P90" s="26"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A91" s="59"/>
-      <c r="B91" s="59"/>
-      <c r="C91" s="56" t="s">
+      <c r="A91" s="51"/>
+      <c r="B91" s="51"/>
+      <c r="C91" s="62" t="s">
         <v>93</v>
       </c>
       <c r="D91" s="21" t="s">
@@ -3730,9 +3620,9 @@
       <c r="P91" s="22"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A92" s="59"/>
-      <c r="B92" s="59"/>
-      <c r="C92" s="57"/>
+      <c r="A92" s="51"/>
+      <c r="B92" s="51"/>
+      <c r="C92" s="63"/>
       <c r="D92" s="21" t="s">
         <v>67</v>
       </c>
@@ -3750,8 +3640,8 @@
       <c r="P92" s="22"/>
     </row>
     <row r="93" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="59"/>
-      <c r="B93" s="59"/>
+      <c r="A93" s="51"/>
+      <c r="B93" s="51"/>
       <c r="C93" s="39"/>
       <c r="D93" s="18"/>
       <c r="E93" s="26"/>
@@ -3768,9 +3658,9 @@
       <c r="P93" s="26"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A94" s="59"/>
-      <c r="B94" s="59"/>
-      <c r="C94" s="58" t="s">
+      <c r="A94" s="51"/>
+      <c r="B94" s="51"/>
+      <c r="C94" s="49" t="s">
         <v>59</v>
       </c>
       <c r="D94" s="21" t="s">
@@ -3790,9 +3680,9 @@
       <c r="P94" s="22"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A95" s="59"/>
-      <c r="B95" s="59"/>
-      <c r="C95" s="58"/>
+      <c r="A95" s="51"/>
+      <c r="B95" s="51"/>
+      <c r="C95" s="49"/>
       <c r="D95" s="21" t="s">
         <v>48</v>
       </c>
@@ -3810,8 +3700,8 @@
       <c r="P95" s="22"/>
     </row>
     <row r="96" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="59"/>
-      <c r="B96" s="59"/>
+      <c r="A96" s="51"/>
+      <c r="B96" s="51"/>
       <c r="C96" s="31"/>
       <c r="D96" s="18"/>
       <c r="E96" s="26"/>
@@ -3828,8 +3718,8 @@
       <c r="P96" s="26"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A97" s="59"/>
-      <c r="B97" s="59"/>
+      <c r="A97" s="51"/>
+      <c r="B97" s="51"/>
       <c r="C97" s="23" t="s">
         <v>88</v>
       </c>
@@ -3884,8 +3774,8 @@
       </c>
     </row>
     <row r="98" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="59"/>
-      <c r="B98" s="59"/>
+      <c r="A98" s="51"/>
+      <c r="B98" s="51"/>
       <c r="C98" s="18"/>
       <c r="D98" s="18"/>
       <c r="E98" s="16"/>
@@ -3902,8 +3792,8 @@
       <c r="P98" s="16"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A99" s="59"/>
-      <c r="B99" s="59"/>
+      <c r="A99" s="51"/>
+      <c r="B99" s="51"/>
       <c r="C99" s="23" t="s">
         <v>94</v>
       </c>
@@ -3976,11 +3866,11 @@
       <c r="P100" s="16"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A101" s="59" t="s">
+      <c r="A101" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B101" s="59"/>
-      <c r="C101" s="58" t="s">
+      <c r="B101" s="51"/>
+      <c r="C101" s="49" t="s">
         <v>68</v>
       </c>
       <c r="D101" s="21" t="s">
@@ -4000,9 +3890,9 @@
       <c r="P101" s="22"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A102" s="59"/>
-      <c r="B102" s="59"/>
-      <c r="C102" s="58"/>
+      <c r="A102" s="51"/>
+      <c r="B102" s="51"/>
+      <c r="C102" s="49"/>
       <c r="D102" s="21" t="s">
         <v>85</v>
       </c>
@@ -4020,9 +3910,9 @@
       <c r="P102" s="22"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A103" s="59"/>
-      <c r="B103" s="59"/>
-      <c r="C103" s="58"/>
+      <c r="A103" s="51"/>
+      <c r="B103" s="51"/>
+      <c r="C103" s="49"/>
       <c r="D103" s="21" t="s">
         <v>86</v>
       </c>
@@ -4040,9 +3930,9 @@
       <c r="P103" s="22"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A104" s="59"/>
-      <c r="B104" s="59"/>
-      <c r="C104" s="58"/>
+      <c r="A104" s="51"/>
+      <c r="B104" s="51"/>
+      <c r="C104" s="49"/>
       <c r="D104" s="21" t="s">
         <v>92</v>
       </c>
@@ -4060,8 +3950,8 @@
       <c r="P104" s="22"/>
     </row>
     <row r="105" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="59"/>
-      <c r="B105" s="59"/>
+      <c r="A105" s="51"/>
+      <c r="B105" s="51"/>
       <c r="C105" s="39"/>
       <c r="D105" s="18"/>
       <c r="E105" s="26"/>
@@ -4078,9 +3968,9 @@
       <c r="P105" s="26"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A106" s="59"/>
-      <c r="B106" s="59"/>
-      <c r="C106" s="58" t="s">
+      <c r="A106" s="51"/>
+      <c r="B106" s="51"/>
+      <c r="C106" s="49" t="s">
         <v>31</v>
       </c>
       <c r="D106" s="21" t="s">
@@ -4100,9 +3990,9 @@
       <c r="P106" s="22"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A107" s="59"/>
-      <c r="B107" s="59"/>
-      <c r="C107" s="58"/>
+      <c r="A107" s="51"/>
+      <c r="B107" s="51"/>
+      <c r="C107" s="49"/>
       <c r="D107" s="21" t="s">
         <v>70</v>
       </c>
@@ -4120,9 +4010,9 @@
       <c r="P107" s="22"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A108" s="59"/>
-      <c r="B108" s="59"/>
-      <c r="C108" s="58"/>
+      <c r="A108" s="51"/>
+      <c r="B108" s="51"/>
+      <c r="C108" s="49"/>
       <c r="D108" s="21" t="s">
         <v>71</v>
       </c>
@@ -4140,8 +4030,8 @@
       <c r="P108" s="22"/>
     </row>
     <row r="109" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="59"/>
-      <c r="B109" s="59"/>
+      <c r="A109" s="51"/>
+      <c r="B109" s="51"/>
       <c r="C109" s="39"/>
       <c r="D109" s="18"/>
       <c r="E109" s="26"/>
@@ -4158,8 +4048,8 @@
       <c r="P109" s="26"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A110" s="59"/>
-      <c r="B110" s="59"/>
+      <c r="A110" s="51"/>
+      <c r="B110" s="51"/>
       <c r="C110" s="38" t="s">
         <v>73</v>
       </c>
@@ -4180,8 +4070,8 @@
       <c r="P110" s="22"/>
     </row>
     <row r="111" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="59"/>
-      <c r="B111" s="59"/>
+      <c r="A111" s="51"/>
+      <c r="B111" s="51"/>
       <c r="C111" s="27"/>
       <c r="D111" s="18"/>
       <c r="E111" s="16"/>
@@ -4198,8 +4088,8 @@
       <c r="P111" s="16"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A112" s="59"/>
-      <c r="B112" s="59"/>
+      <c r="A112" s="51"/>
+      <c r="B112" s="51"/>
       <c r="C112" s="23" t="s">
         <v>96</v>
       </c>
@@ -4254,8 +4144,8 @@
       </c>
     </row>
     <row r="113" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="59"/>
-      <c r="B113" s="59"/>
+      <c r="A113" s="51"/>
+      <c r="B113" s="51"/>
       <c r="C113" s="18"/>
       <c r="D113" s="18"/>
       <c r="E113" s="16"/>
@@ -4272,8 +4162,8 @@
       <c r="P113" s="16"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A114" s="59"/>
-      <c r="B114" s="59"/>
+      <c r="A114" s="51"/>
+      <c r="B114" s="51"/>
       <c r="C114" s="23" t="s">
         <v>94</v>
       </c>
@@ -4344,11 +4234,11 @@
       <c r="P115" s="16"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A116" s="47" t="s">
+      <c r="A116" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="B116" s="48"/>
-      <c r="C116" s="49"/>
+      <c r="B116" s="55"/>
+      <c r="C116" s="56"/>
       <c r="D116" s="32" t="s">
         <v>0</v>
       </c>
@@ -4402,9 +4292,9 @@
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A117" s="50"/>
-      <c r="B117" s="51"/>
-      <c r="C117" s="52"/>
+      <c r="A117" s="57"/>
+      <c r="B117" s="52"/>
+      <c r="C117" s="58"/>
       <c r="D117" s="32" t="s">
         <v>23</v>
       </c>
@@ -4458,9 +4348,9 @@
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A118" s="50"/>
-      <c r="B118" s="51"/>
-      <c r="C118" s="52"/>
+      <c r="A118" s="57"/>
+      <c r="B118" s="52"/>
+      <c r="C118" s="58"/>
       <c r="D118" s="32" t="s">
         <v>89</v>
       </c>
@@ -4514,9 +4404,9 @@
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A119" s="50"/>
-      <c r="B119" s="51"/>
-      <c r="C119" s="52"/>
+      <c r="A119" s="57"/>
+      <c r="B119" s="52"/>
+      <c r="C119" s="58"/>
       <c r="D119" s="32" t="s">
         <v>90</v>
       </c>
@@ -4570,9 +4460,9 @@
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A120" s="50"/>
-      <c r="B120" s="51"/>
-      <c r="C120" s="52"/>
+      <c r="A120" s="57"/>
+      <c r="B120" s="52"/>
+      <c r="C120" s="58"/>
       <c r="D120" s="32" t="s">
         <v>91</v>
       </c>
@@ -4626,9 +4516,9 @@
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A121" s="50"/>
-      <c r="B121" s="51"/>
-      <c r="C121" s="52"/>
+      <c r="A121" s="57"/>
+      <c r="B121" s="52"/>
+      <c r="C121" s="58"/>
       <c r="D121" s="32" t="s">
         <v>95</v>
       </c>
@@ -4682,9 +4572,9 @@
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A122" s="53"/>
-      <c r="B122" s="54"/>
-      <c r="C122" s="55"/>
+      <c r="A122" s="59"/>
+      <c r="B122" s="60"/>
+      <c r="C122" s="61"/>
       <c r="D122" s="45" t="s">
         <v>46</v>
       </c>
@@ -4760,13 +4650,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A7:C15"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="A31:B56"/>
-    <mergeCell ref="A19:C27"/>
-    <mergeCell ref="A16:C18"/>
-    <mergeCell ref="A28:C30"/>
     <mergeCell ref="A116:C122"/>
     <mergeCell ref="C91:C92"/>
     <mergeCell ref="C94:C95"/>
@@ -4783,6 +4666,13 @@
     <mergeCell ref="A58:B85"/>
     <mergeCell ref="A87:B99"/>
     <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A7:C15"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="A31:B56"/>
+    <mergeCell ref="A19:C27"/>
+    <mergeCell ref="A16:C18"/>
+    <mergeCell ref="A28:C30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E122:P122">

</xml_diff>